<commit_message>
Fixed excel file and import command.
</commit_message>
<xml_diff>
--- a/data-import/news_articles.xlsx
+++ b/data-import/news_articles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\dejan92\pimcoretask\task\data-import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB63F6C-87E5-400E-88B8-0C78E2C47E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1303908-C6E4-497B-910B-6F545310CB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A93960A2-E1FB-44F5-8C89-95FBA9842F79}"/>
   </bookViews>
@@ -36,37 +36,114 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="4">
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>author</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>J.R.R. Tolkien</t>
   </si>
   <si>
-    <t>key</t>
+    <t>Sword Catcher</t>
+  </si>
+  <si>
+    <t>Cassandra Clare</t>
+  </si>
+  <si>
+    <t>Wheel of Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robert Jordan </t>
+  </si>
+  <si>
+    <t>The Lord of the Rings</t>
+  </si>
+  <si>
+    <t>George R.R. Martin</t>
+  </si>
+  <si>
+    <t>A Game of Thrones</t>
+  </si>
+  <si>
+    <t>Brandon Sanderson</t>
+  </si>
+  <si>
+    <t>The Stormlight Archive</t>
+  </si>
+  <si>
+    <t>Patrick Rothfuss</t>
+  </si>
+  <si>
+    <t>The Kingkiller Chronicle</t>
+  </si>
+  <si>
+    <t>C.S. Lewis</t>
+  </si>
+  <si>
+    <t>The Chronicles of Narnia</t>
+  </si>
+  <si>
+    <t>Stephen King</t>
+  </si>
+  <si>
+    <t>The Dark Tower</t>
+  </si>
+  <si>
+    <t>Ursula Le Guin</t>
+  </si>
+  <si>
+    <t>A Wizard of Earthsea</t>
+  </si>
+  <si>
+    <t>Nnedi Okorafor</t>
+  </si>
+  <si>
+    <t>Who Fears Death</t>
+  </si>
+  <si>
+    <t>Robin Hobb</t>
+  </si>
+  <si>
+    <t>The Farseer Trilogy</t>
+  </si>
+  <si>
+    <t>Fonda Lee</t>
+  </si>
+  <si>
+    <t>Jade City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frank Herbert </t>
+  </si>
+  <si>
+    <t>Dune</t>
+  </si>
+  <si>
+    <t>J.K Rowling</t>
+  </si>
+  <si>
+    <t>Harry Potter</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Neque porro quisquam est qui dolorem ipsum quia dolor sit amet, consectetur, adipisci velit..."
+"There is no one who loves pain itself, who seeks after it and wants to have it, simply because it is pain..."</t>
+  </si>
+  <si>
+    <t>J.R.R. Neque porro quisquam est qui dolorem ipsum quia dolor sit amet, consectetur, adipisci velit..."
+"There is no one who loves pain itself, who seeks after it and wants to have it, simply because it is pain..."</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FFBDC1C6"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,17 +166,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -415,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77193C4B-E9E2-4851-B9B6-2E0D795B27AB}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,195 +499,203 @@
     <col min="1" max="1" width="19.44140625" customWidth="1"/>
     <col min="2" max="2" width="43.77734375" customWidth="1"/>
     <col min="3" max="3" width="26.21875" customWidth="1"/>
+    <col min="4" max="4" width="34" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" t="s">
-        <v>2</v>
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>